<commit_message>
1. new regular results 2. new results variable, future TODO: write it to output, collect it when creating results file
</commit_message>
<xml_diff>
--- a/GeneratedProblems_Regular/Resutls/results_regular.xlsx
+++ b/GeneratedProblems_Regular/Resutls/results_regular.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="6525" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -1906,11 +1906,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="649795664"/>
-        <c:axId val="649789392"/>
+        <c:axId val="813366328"/>
+        <c:axId val="813362800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="649795664"/>
+        <c:axId val="813366328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,7 +2013,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649789392"/>
+        <c:crossAx val="813362800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2021,7 +2021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="649789392"/>
+        <c:axId val="813362800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649795664"/>
+        <c:crossAx val="813366328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2295,7 +2295,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -2539,11 +2538,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="649789784"/>
-        <c:axId val="649790568"/>
+        <c:axId val="813365544"/>
+        <c:axId val="813363192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="649789784"/>
+        <c:axId val="813365544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,14 +2570,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="649790568"/>
+        <c:crossAx val="813363192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2586,7 +2584,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="649790568"/>
+        <c:axId val="813363192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2614,14 +2612,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="649789784"/>
+        <c:crossAx val="813365544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2953,11 +2950,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="649791744"/>
-        <c:axId val="649792920"/>
+        <c:axId val="813364368"/>
+        <c:axId val="897495576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="649791744"/>
+        <c:axId val="813364368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2992,7 +2989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="649792920"/>
+        <c:crossAx val="897495576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3000,7 +2997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="649792920"/>
+        <c:axId val="897495576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,7 +3032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="649791744"/>
+        <c:crossAx val="813364368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3589,11 +3586,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="349362376"/>
-        <c:axId val="349363944"/>
+        <c:axId val="897490872"/>
+        <c:axId val="897494792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="349362376"/>
+        <c:axId val="897490872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3692,7 +3689,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349363944"/>
+        <c:crossAx val="897494792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3700,7 +3697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349363944"/>
+        <c:axId val="897494792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3812,7 +3809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349362376"/>
+        <c:crossAx val="897490872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5382,11 +5379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S321"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R321" sqref="R145:R321"/>
+    <sheetView tabSelected="1" topLeftCell="J302" workbookViewId="0">
+      <selection activeCell="T309" sqref="T309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5467,7 +5463,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5529,7 +5525,7 @@
         <v>-0.65999960899352184</v>
       </c>
     </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5591,7 +5587,7 @@
         <v>0.69100022315978182</v>
       </c>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5653,7 +5649,7 @@
         <v>1.2389998435974081</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5715,7 +5711,7 @@
         <v>-5.5999999046325657</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5777,7 +5773,7 @@
         <v>0.25100016593932523</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5839,7 +5835,7 @@
         <v>8.0000162124631791E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5901,7 +5897,7 @@
         <v>0.31900000572204423</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5963,7 +5959,7 @@
         <v>0.33399987220764227</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6025,7 +6021,7 @@
         <v>0.47500038146972734</v>
       </c>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6087,7 +6083,7 @@
         <v>-11.038000106811465</v>
       </c>
     </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6149,7 +6145,7 @@
         <v>-4.8669998645782488</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -6211,7 +6207,7 @@
         <v>1.7769999504089344</v>
       </c>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -6273,7 +6269,7 @@
         <v>0.7380001544952377</v>
       </c>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -6335,7 +6331,7 @@
         <v>-1.3980000019073442</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -6397,7 +6393,7 @@
         <v>0.93000030517578258</v>
       </c>
     </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -6459,7 +6455,7 @@
         <v>1.5059998035430964</v>
       </c>
     </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -6521,7 +6517,7 @@
         <v>-23.424000024795468</v>
       </c>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -6583,7 +6579,7 @@
         <v>1.128999710083016</v>
       </c>
     </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -6645,7 +6641,7 @@
         <v>-1.6080000400543129</v>
       </c>
     </row>
-    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -6707,7 +6703,7 @@
         <v>2.334000110626226</v>
       </c>
     </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -6769,7 +6765,7 @@
         <v>13.483000040054296</v>
       </c>
     </row>
-    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -6831,7 +6827,7 @@
         <v>4.7259998321533114</v>
       </c>
     </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -6893,7 +6889,7 @@
         <v>23.923999786376921</v>
       </c>
     </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -6955,7 +6951,7 @@
         <v>8.8009998798369971</v>
       </c>
     </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -7017,7 +7013,7 @@
         <v>4.5439996719359668</v>
       </c>
     </row>
-    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -7079,7 +7075,7 @@
         <v>9.8689999580382732</v>
       </c>
     </row>
-    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -7141,7 +7137,7 @@
         <v>25.934000015258718</v>
       </c>
     </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -7203,7 +7199,7 @@
         <v>7.062999963760376</v>
       </c>
     </row>
-    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -7265,7 +7261,7 @@
         <v>10.387000083923285</v>
       </c>
     </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -7327,7 +7323,7 @@
         <v>5.2289998531340594</v>
       </c>
     </row>
-    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -7389,7 +7385,7 @@
         <v>44.25099992752078</v>
       </c>
     </row>
-    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -7451,7 +7447,7 @@
         <v>61.945999860763571</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -7513,7 +7509,7 @@
         <v>25.53799986839293</v>
       </c>
     </row>
-    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -7575,7 +7571,7 @@
         <v>52.583000183105398</v>
       </c>
     </row>
-    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -7637,7 +7633,7 @@
         <v>62.279999971389785</v>
       </c>
     </row>
-    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -7699,7 +7695,7 @@
         <v>24.067999839782782</v>
       </c>
     </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -7761,7 +7757,7 @@
         <v>28.379000186920102</v>
       </c>
     </row>
-    <row r="39" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -7823,7 +7819,7 @@
         <v>27.137999773025538</v>
       </c>
     </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -7885,7 +7881,7 @@
         <v>31.881999969482415</v>
       </c>
     </row>
-    <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -7947,7 +7943,7 @@
         <v>11.721000194549614</v>
       </c>
     </row>
-    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -8009,7 +8005,7 @@
         <v>0.75100016593932339</v>
       </c>
     </row>
-    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -8071,7 +8067,7 @@
         <v>0.61099982261656915</v>
       </c>
     </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -8133,7 +8129,7 @@
         <v>0.65799999237059614</v>
       </c>
     </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -8195,7 +8191,7 @@
         <v>0.47700023651122431</v>
       </c>
     </row>
-    <row r="46" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -8257,7 +8253,7 @@
         <v>1.6740000247955265</v>
       </c>
     </row>
-    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -8319,7 +8315,7 @@
         <v>0.55199980735778842</v>
       </c>
     </row>
-    <row r="48" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -8381,7 +8377,7 @@
         <v>-0.46299982070923451</v>
       </c>
     </row>
-    <row r="49" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -8443,7 +8439,7 @@
         <v>0.74099993705748735</v>
       </c>
     </row>
-    <row r="50" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -8505,7 +8501,7 @@
         <v>-0.98399996757507457</v>
       </c>
     </row>
-    <row r="51" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -8567,7 +8563,7 @@
         <v>0.17700004577635853</v>
       </c>
     </row>
-    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -8629,7 +8625,7 @@
         <v>1.4650001525878897</v>
       </c>
     </row>
-    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -8691,7 +8687,7 @@
         <v>2.3970000743865976</v>
       </c>
     </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -8753,7 +8749,7 @@
         <v>2.9879999160766588</v>
       </c>
     </row>
-    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -8815,7 +8811,7 @@
         <v>0.66600012779236217</v>
       </c>
     </row>
-    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -8877,7 +8873,7 @@
         <v>1.257000207901007</v>
       </c>
     </row>
-    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -8939,7 +8935,7 @@
         <v>1.976000070571895</v>
       </c>
     </row>
-    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -9001,7 +8997,7 @@
         <v>1.7129998207092303</v>
       </c>
     </row>
-    <row r="59" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -9063,7 +9059,7 @@
         <v>3.3509998321533234</v>
       </c>
     </row>
-    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -9125,7 +9121,7 @@
         <v>1.1040000915527366</v>
       </c>
     </row>
-    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -9187,7 +9183,7 @@
         <v>1.8129999637603804</v>
       </c>
     </row>
-    <row r="62" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -9249,7 +9245,7 @@
         <v>5.2969999313354306</v>
       </c>
     </row>
-    <row r="63" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -9311,7 +9307,7 @@
         <v>14.149999856948831</v>
       </c>
     </row>
-    <row r="64" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -9373,7 +9369,7 @@
         <v>6.888000011444066</v>
       </c>
     </row>
-    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -9435,7 +9431,7 @@
         <v>14.684999942779541</v>
       </c>
     </row>
-    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -9497,7 +9493,7 @@
         <v>6.5650000572203959</v>
       </c>
     </row>
-    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -9559,7 +9555,7 @@
         <v>12.476000070571887</v>
       </c>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -9621,7 +9617,7 @@
         <v>9.5080001354216854</v>
       </c>
     </row>
-    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -9683,7 +9679,7 @@
         <v>-14.534000158309894</v>
       </c>
     </row>
-    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -9745,7 +9741,7 @@
         <v>10.42000007629386</v>
       </c>
     </row>
-    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -9807,7 +9803,7 @@
         <v>6.4769999980925688</v>
       </c>
     </row>
-    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -9869,7 +9865,7 @@
         <v>43.220000028610173</v>
       </c>
     </row>
-    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -9931,7 +9927,7 @@
         <v>12.665000200271573</v>
       </c>
     </row>
-    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -9993,7 +9989,7 @@
         <v>43.171999931335492</v>
       </c>
     </row>
-    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -10055,7 +10051,7 @@
         <v>39.834999799728458</v>
       </c>
     </row>
-    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -10117,7 +10113,7 @@
         <v>1512.2340002059925</v>
       </c>
     </row>
-    <row r="77" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -10179,7 +10175,7 @@
         <v>17.467999935150157</v>
       </c>
     </row>
-    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -10241,7 +10237,7 @@
         <v>76.858000040054293</v>
       </c>
     </row>
-    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -10303,7 +10299,7 @@
         <v>103.26700019836422</v>
       </c>
     </row>
-    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -10365,7 +10361,7 @@
         <v>21.17100000381469</v>
       </c>
     </row>
-    <row r="81" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -10427,7 +10423,7 @@
         <v>259.18499994277943</v>
       </c>
     </row>
-    <row r="82" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -10488,7 +10484,7 @@
         <v>-1792.8760001659393</v>
       </c>
     </row>
-    <row r="83" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -10550,7 +10546,7 @@
         <v>-82.624999999999972</v>
       </c>
     </row>
-    <row r="84" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -10612,7 +10608,7 @@
         <v>-524.73600006103516</v>
       </c>
     </row>
-    <row r="85" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -10674,7 +10670,7 @@
         <v>-734.00800013542164</v>
       </c>
     </row>
-    <row r="86" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -10735,7 +10731,7 @@
         <v>-1797.8310000896454</v>
       </c>
     </row>
-    <row r="87" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -10796,7 +10792,7 @@
         <v>-1797.8980000019073</v>
       </c>
     </row>
-    <row r="88" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -10858,7 +10854,7 @@
         <v>-441.73999977111754</v>
       </c>
     </row>
-    <row r="89" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -10920,7 +10916,7 @@
         <v>-1391.9260001182515</v>
       </c>
     </row>
-    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -10981,7 +10977,7 @@
         <v>-1792.4340000152588</v>
       </c>
     </row>
-    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -11043,7 +11039,7 @@
         <v>-56.028000116348196</v>
       </c>
     </row>
-    <row r="92" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -11104,7 +11100,7 @@
         <v>-1780.8819999694824</v>
       </c>
     </row>
-    <row r="93" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -11166,7 +11162,7 @@
         <v>-233.14200019836343</v>
       </c>
     </row>
-    <row r="94" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -11227,7 +11223,7 @@
         <v>-1785.5900001525879</v>
       </c>
     </row>
-    <row r="95" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -11288,7 +11284,7 @@
         <v>-1778.7579998970032</v>
       </c>
     </row>
-    <row r="96" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -11349,7 +11345,7 @@
         <v>-1775.0069999694824</v>
       </c>
     </row>
-    <row r="97" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -11411,7 +11407,7 @@
         <v>-69.727999925613389</v>
       </c>
     </row>
-    <row r="98" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -11473,7 +11469,7 @@
         <v>-389.2569997310631</v>
       </c>
     </row>
-    <row r="99" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -11534,7 +11530,7 @@
         <v>-1779.0149998664856</v>
       </c>
     </row>
-    <row r="100" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -11596,7 +11592,7 @@
         <v>0.24000000953668987</v>
       </c>
     </row>
-    <row r="101" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -11658,7 +11654,7 @@
         <v>-562.7409999370575</v>
       </c>
     </row>
-    <row r="102" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -11720,7 +11716,7 @@
         <v>-3.7650001049041535</v>
       </c>
     </row>
-    <row r="103" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -11782,7 +11778,7 @@
         <v>-6.3120000362395672</v>
       </c>
     </row>
-    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -11844,7 +11840,7 @@
         <v>19.036000013351575</v>
       </c>
     </row>
-    <row r="105" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -11906,7 +11902,7 @@
         <v>-757.59599971771229</v>
       </c>
     </row>
-    <row r="106" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -11968,7 +11964,7 @@
         <v>-74.200999975203516</v>
       </c>
     </row>
-    <row r="107" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -12030,7 +12026,7 @@
         <v>-98.980999946593357</v>
       </c>
     </row>
-    <row r="108" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -12092,7 +12088,7 @@
         <v>-335.62300014495804</v>
       </c>
     </row>
-    <row r="109" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -12153,7 +12149,7 @@
         <v>-1741.0569999217987</v>
       </c>
     </row>
-    <row r="110" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -12214,7 +12210,7 @@
         <v>-1699.0489997863772</v>
       </c>
     </row>
-    <row r="111" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -12276,7 +12272,7 @@
         <v>8.656000137329066</v>
       </c>
     </row>
-    <row r="112" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -12338,7 +12334,7 @@
         <v>-317.32499980926525</v>
       </c>
     </row>
-    <row r="113" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -12400,7 +12396,7 @@
         <v>191.59899997711165</v>
       </c>
     </row>
-    <row r="114" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -12462,7 +12458,7 @@
         <v>333.6360001564031</v>
       </c>
     </row>
-    <row r="115" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -12523,7 +12519,7 @@
         <v>-1555.6010000705724</v>
       </c>
     </row>
-    <row r="116" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -12585,7 +12581,7 @@
         <v>265.31800007820061</v>
       </c>
     </row>
-    <row r="117" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -12647,7 +12643,7 @@
         <v>295.70799994468604</v>
       </c>
     </row>
-    <row r="118" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -12709,7 +12705,7 @@
         <v>61.878000020980309</v>
       </c>
     </row>
-    <row r="119" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -12771,7 +12767,7 @@
         <v>-864.64600014685846</v>
       </c>
     </row>
-    <row r="120" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -12833,7 +12829,7 @@
         <v>-1339.2569999694831</v>
       </c>
     </row>
-    <row r="121" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -12895,7 +12891,7 @@
         <v>168.7119996547695</v>
       </c>
     </row>
-    <row r="122" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -12957,7 +12953,7 @@
         <v>-2.3959996700286843</v>
       </c>
     </row>
-    <row r="123" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -13019,7 +13015,7 @@
         <v>-281.83700013160615</v>
       </c>
     </row>
-    <row r="124" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -13081,7 +13077,7 @@
         <v>-38.594000101089428</v>
       </c>
     </row>
-    <row r="125" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -13143,7 +13139,7 @@
         <v>-79.455999612808228</v>
       </c>
     </row>
-    <row r="126" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -13205,7 +13201,7 @@
         <v>-417.53200006484985</v>
       </c>
     </row>
-    <row r="127" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -13267,7 +13263,7 @@
         <v>-1087.7990000247898</v>
       </c>
     </row>
-    <row r="128" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -13328,7 +13324,7 @@
         <v>-1797.194000005722</v>
       </c>
     </row>
-    <row r="129" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -13390,7 +13386,7 @@
         <v>-31.733000040054296</v>
       </c>
     </row>
-    <row r="130" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -13452,7 +13448,7 @@
         <v>-537.04500007629315</v>
       </c>
     </row>
-    <row r="131" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -13514,7 +13510,7 @@
         <v>-47.636999845504675</v>
       </c>
     </row>
-    <row r="132" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -13576,7 +13572,7 @@
         <v>-165.34400033950757</v>
       </c>
     </row>
-    <row r="133" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -13637,7 +13633,7 @@
         <v>-1791.9980001449585</v>
       </c>
     </row>
-    <row r="134" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -13698,7 +13694,7 @@
         <v>-1769.6579999923706</v>
       </c>
     </row>
-    <row r="135" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -13760,7 +13756,7 @@
         <v>-37.666999816894474</v>
       </c>
     </row>
-    <row r="136" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -13821,7 +13817,7 @@
         <v>-1757.0010001659393</v>
       </c>
     </row>
-    <row r="137" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -13883,7 +13879,7 @@
         <v>-200.06599974632257</v>
       </c>
     </row>
-    <row r="138" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -13945,7 +13941,7 @@
         <v>-663.31099987030007</v>
       </c>
     </row>
-    <row r="139" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -14006,7 +14002,7 @@
         <v>-1778.0019998550415</v>
       </c>
     </row>
-    <row r="140" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -14068,7 +14064,7 @@
         <v>-328.04099988937321</v>
       </c>
     </row>
-    <row r="141" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -14130,7 +14126,7 @@
         <v>-883.78499984741131</v>
       </c>
     </row>
-    <row r="142" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -14192,7 +14188,7 @@
         <v>-84.751999855041603</v>
       </c>
     </row>
-    <row r="143" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -14254,7 +14250,7 @@
         <v>182.36299991607586</v>
       </c>
     </row>
-    <row r="144" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -14378,7 +14374,7 @@
         <v>1620.7730000019083</v>
       </c>
     </row>
-    <row r="146" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -14440,7 +14436,7 @@
         <v>-159.75299978256169</v>
       </c>
     </row>
-    <row r="147" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -14502,7 +14498,7 @@
         <v>-415.79399991035444</v>
       </c>
     </row>
-    <row r="148" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -14564,7 +14560,7 @@
         <v>-333.15999984741256</v>
       </c>
     </row>
-    <row r="149" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -14626,7 +14622,7 @@
         <v>-832.78600001334451</v>
       </c>
     </row>
-    <row r="150" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -14687,7 +14683,7 @@
         <v>-1667.914999961853</v>
       </c>
     </row>
-    <row r="151" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -14749,7 +14745,7 @@
         <v>-27.191999912262048</v>
       </c>
     </row>
-    <row r="152" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -14810,7 +14806,7 @@
         <v>-1631.1359999179845</v>
       </c>
     </row>
-    <row r="153" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -14872,7 +14868,7 @@
         <v>-46.3990001678456</v>
       </c>
     </row>
-    <row r="154" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -14934,7 +14930,7 @@
         <v>-126.32900023460303</v>
       </c>
     </row>
-    <row r="155" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -14995,7 +14991,7 @@
         <v>-1526.2839996814732</v>
       </c>
     </row>
-    <row r="156" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -15118,7 +15114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -15179,7 +15175,7 @@
         <v>-1578.677999734879</v>
       </c>
     </row>
-    <row r="159" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -15240,7 +15236,7 @@
         <v>-96.809000015264473</v>
       </c>
     </row>
-    <row r="160" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -15302,7 +15298,7 @@
         <v>430.03199982643179</v>
       </c>
     </row>
-    <row r="161" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -15364,7 +15360,7 @@
         <v>162.49100017547593</v>
       </c>
     </row>
-    <row r="162" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -15426,7 +15422,7 @@
         <v>1.3590002059936528</v>
       </c>
     </row>
-    <row r="163" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -15488,7 +15484,7 @@
         <v>-5.1520001888275146</v>
       </c>
     </row>
-    <row r="164" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -15550,7 +15546,7 @@
         <v>1.9940001964569134</v>
       </c>
     </row>
-    <row r="165" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -15612,7 +15608,7 @@
         <v>1.2170000076293985</v>
       </c>
     </row>
-    <row r="166" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -15674,7 +15670,7 @@
         <v>1.8499999046325712</v>
       </c>
     </row>
-    <row r="167" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -15736,7 +15732,7 @@
         <v>1.5789999961853054</v>
       </c>
     </row>
-    <row r="168" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -15798,7 +15794,7 @@
         <v>1.5690002441406234</v>
       </c>
     </row>
-    <row r="169" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -15860,7 +15856,7 @@
         <v>-0.5839998722076436</v>
       </c>
     </row>
-    <row r="170" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -15922,7 +15918,7 @@
         <v>0.95500016212463246</v>
       </c>
     </row>
-    <row r="171" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -15984,7 +15980,7 @@
         <v>1.0580003261566162</v>
       </c>
     </row>
-    <row r="172" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -16046,7 +16042,7 @@
         <v>10.696999788284296</v>
       </c>
     </row>
-    <row r="173" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -16108,7 +16104,7 @@
         <v>6.0759999752044376</v>
       </c>
     </row>
-    <row r="174" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -16170,7 +16166,7 @@
         <v>5.3659999370574596</v>
       </c>
     </row>
-    <row r="175" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -16232,7 +16228,7 @@
         <v>9.879000186920166</v>
       </c>
     </row>
-    <row r="176" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -16294,7 +16290,7 @@
         <v>-9.597999811172464</v>
       </c>
     </row>
-    <row r="177" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -16356,7 +16352,7 @@
         <v>11.345999956130981</v>
       </c>
     </row>
-    <row r="178" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -16418,7 +16414,7 @@
         <v>11.824000120162889</v>
       </c>
     </row>
-    <row r="179" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -16480,7 +16476,7 @@
         <v>6.3569998741148961</v>
       </c>
     </row>
-    <row r="180" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -16542,7 +16538,7 @@
         <v>4.1519999504089418</v>
       </c>
     </row>
-    <row r="181" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -16604,7 +16600,7 @@
         <v>5.4059998989104354</v>
       </c>
     </row>
-    <row r="182" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -16666,7 +16662,7 @@
         <v>32.444000244140618</v>
       </c>
     </row>
-    <row r="183" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -16728,7 +16724,7 @@
         <v>30.562000036239617</v>
       </c>
     </row>
-    <row r="184" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -16790,7 +16786,7 @@
         <v>86.311000108718773</v>
       </c>
     </row>
-    <row r="185" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -16852,7 +16848,7 @@
         <v>16.836000204086286</v>
       </c>
     </row>
-    <row r="186" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -16914,7 +16910,7 @@
         <v>151.73699998855565</v>
       </c>
     </row>
-    <row r="187" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -16976,7 +16972,7 @@
         <v>37.486000061035114</v>
       </c>
     </row>
-    <row r="188" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -17038,7 +17034,7 @@
         <v>22.984000205993659</v>
       </c>
     </row>
-    <row r="189" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -17100,7 +17096,7 @@
         <v>15.523999929428166</v>
       </c>
     </row>
-    <row r="190" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -17162,7 +17158,7 @@
         <v>18.046000003814676</v>
       </c>
     </row>
-    <row r="191" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -17224,7 +17220,7 @@
         <v>61.30200004577641</v>
       </c>
     </row>
-    <row r="192" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -17286,7 +17282,7 @@
         <v>172.40699982643065</v>
       </c>
     </row>
-    <row r="193" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -17348,7 +17344,7 @@
         <v>206.62900018691923</v>
       </c>
     </row>
-    <row r="194" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -17410,7 +17406,7 @@
         <v>78.455000162124151</v>
       </c>
     </row>
-    <row r="195" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -17472,7 +17468,7 @@
         <v>191.49899983406061</v>
       </c>
     </row>
-    <row r="196" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -17534,7 +17530,7 @@
         <v>142.49300003051752</v>
       </c>
     </row>
-    <row r="197" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -17596,7 +17592,7 @@
         <v>302.75800013542118</v>
       </c>
     </row>
-    <row r="198" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -17658,7 +17654,7 @@
         <v>284.81100010871864</v>
       </c>
     </row>
-    <row r="199" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -17720,7 +17716,7 @@
         <v>58.573000431060734</v>
       </c>
     </row>
-    <row r="200" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -17782,7 +17778,7 @@
         <v>71.20000004768346</v>
       </c>
     </row>
-    <row r="201" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -17844,7 +17840,7 @@
         <v>58.17300009727478</v>
       </c>
     </row>
-    <row r="202" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -17906,7 +17902,7 @@
         <v>5.0000190734857175E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -17968,7 +17964,7 @@
         <v>1.494999647140504</v>
       </c>
     </row>
-    <row r="204" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -18030,7 +18026,7 @@
         <v>1.6789996623992947</v>
       </c>
     </row>
-    <row r="205" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -18092,7 +18088,7 @@
         <v>79.36499977111815</v>
       </c>
     </row>
-    <row r="206" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -18154,7 +18150,7 @@
         <v>2.205000162124632</v>
       </c>
     </row>
-    <row r="207" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -18216,7 +18212,7 @@
         <v>2.2030000686645548</v>
       </c>
     </row>
-    <row r="208" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -18278,7 +18274,7 @@
         <v>0.53500032424927557</v>
       </c>
     </row>
-    <row r="209" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -18340,7 +18336,7 @@
         <v>1.242999792099007</v>
       </c>
     </row>
-    <row r="210" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -18402,7 +18398,7 @@
         <v>1.4449996948242165</v>
       </c>
     </row>
-    <row r="211" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -18464,7 +18460,7 @@
         <v>1.8199999332428005</v>
       </c>
     </row>
-    <row r="212" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -18526,7 +18522,7 @@
         <v>3.3639998435974157</v>
       </c>
     </row>
-    <row r="213" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -18588,7 +18584,7 @@
         <v>4.7899999618530309</v>
       </c>
     </row>
-    <row r="214" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -18650,7 +18646,7 @@
         <v>8.7849998474121165</v>
       </c>
     </row>
-    <row r="215" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -18712,7 +18708,7 @@
         <v>4.9979996681213077</v>
       </c>
     </row>
-    <row r="216" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -18774,7 +18770,7 @@
         <v>5.8519999980925856</v>
       </c>
     </row>
-    <row r="217" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -18836,7 +18832,7 @@
         <v>11.536000013351426</v>
       </c>
     </row>
-    <row r="218" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -18898,7 +18894,7 @@
         <v>5.6900000572203835</v>
       </c>
     </row>
-    <row r="219" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -18960,7 +18956,7 @@
         <v>8.9320001602172798</v>
       </c>
     </row>
-    <row r="220" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -19022,7 +19018,7 @@
         <v>5.6940002441406232</v>
       </c>
     </row>
-    <row r="221" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -19084,7 +19080,7 @@
         <v>5.8869998455047234</v>
       </c>
     </row>
-    <row r="222" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -19146,7 +19142,7 @@
         <v>28.863000154495232</v>
       </c>
     </row>
-    <row r="223" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -19208,7 +19204,7 @@
         <v>19.780999898910522</v>
       </c>
     </row>
-    <row r="224" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -19270,7 +19266,7 @@
         <v>12.952000141143738</v>
       </c>
     </row>
-    <row r="225" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -19332,7 +19328,7 @@
         <v>113.55200004577638</v>
       </c>
     </row>
-    <row r="226" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -19394,7 +19390,7 @@
         <v>44.308000087738037</v>
       </c>
     </row>
-    <row r="227" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -19456,7 +19452,7 @@
         <v>36.592000007629423</v>
       </c>
     </row>
-    <row r="228" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -19518,7 +19514,7 @@
         <v>61.569000005722067</v>
       </c>
     </row>
-    <row r="229" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -19580,7 +19576,7 @@
         <v>17.932000160217246</v>
       </c>
     </row>
-    <row r="230" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -19642,7 +19638,7 @@
         <v>13.779999971389806</v>
       </c>
     </row>
-    <row r="231" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -19704,7 +19700,7 @@
         <v>43.771999835968025</v>
       </c>
     </row>
-    <row r="232" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -19766,7 +19762,7 @@
         <v>97.096999883651762</v>
       </c>
     </row>
-    <row r="233" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -19828,7 +19824,7 @@
         <v>347.70799994468632</v>
       </c>
     </row>
-    <row r="234" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -19890,7 +19886,7 @@
         <v>64.804999828337742</v>
       </c>
     </row>
-    <row r="235" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -19952,7 +19948,7 @@
         <v>249.05900001525856</v>
       </c>
     </row>
-    <row r="236" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -20014,7 +20010,7 @@
         <v>90.690999984740415</v>
       </c>
     </row>
-    <row r="237" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -20138,7 +20134,7 @@
         <v>1799.3759999275208</v>
       </c>
     </row>
-    <row r="239" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -20200,7 +20196,7 @@
         <v>271.85700011253323</v>
       </c>
     </row>
-    <row r="240" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -20262,7 +20258,7 @@
         <v>32.032000064849782</v>
       </c>
     </row>
-    <row r="241" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -20324,7 +20320,7 @@
         <v>147.56599998474087</v>
       </c>
     </row>
-    <row r="242" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -20447,7 +20443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -20509,7 +20505,7 @@
         <v>-289.15500020980835</v>
       </c>
     </row>
-    <row r="245" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -20571,7 +20567,7 @@
         <v>-9.8250000476837389</v>
       </c>
     </row>
-    <row r="246" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -20632,7 +20628,7 @@
         <v>-1795.7620000839233</v>
       </c>
     </row>
-    <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -20694,7 +20690,7 @@
         <v>-99.725000143051034</v>
       </c>
     </row>
-    <row r="248" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -20756,7 +20752,7 @@
         <v>-209.02000021934475</v>
       </c>
     </row>
-    <row r="249" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -20818,7 +20814,7 @@
         <v>-714.75600004196099</v>
       </c>
     </row>
-    <row r="250" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -20880,7 +20876,7 @@
         <v>-30.739999771118093</v>
       </c>
     </row>
-    <row r="251" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -20941,7 +20937,7 @@
         <v>-1793.4509999752045</v>
       </c>
     </row>
-    <row r="252" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -21003,7 +20999,7 @@
         <v>-462.73600006103482</v>
       </c>
     </row>
-    <row r="253" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -21065,7 +21061,7 @@
         <v>-1000.6029999256059</v>
       </c>
     </row>
-    <row r="254" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -21126,7 +21122,7 @@
         <v>-1750.0130000114441</v>
       </c>
     </row>
-    <row r="255" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -21188,7 +21184,7 @@
         <v>-70.017000198364002</v>
       </c>
     </row>
-    <row r="256" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -21249,7 +21245,7 @@
         <v>-1669.5139999389648</v>
       </c>
     </row>
-    <row r="257" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -21310,7 +21306,7 @@
         <v>-1281.2639999389658</v>
       </c>
     </row>
-    <row r="258" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -21372,7 +21368,7 @@
         <v>1164.5069999694783</v>
       </c>
     </row>
-    <row r="259" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -21434,7 +21430,7 @@
         <v>-133.64499998092637</v>
       </c>
     </row>
-    <row r="260" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -21496,7 +21492,7 @@
         <v>19.8010001182557</v>
       </c>
     </row>
-    <row r="261" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -21619,7 +21615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -21681,7 +21677,7 @@
         <v>217.99600005149784</v>
       </c>
     </row>
-    <row r="264" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -21743,7 +21739,7 @@
         <v>285.63700008392334</v>
       </c>
     </row>
-    <row r="265" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -21805,7 +21801,7 @@
         <v>1411.1000003814686</v>
       </c>
     </row>
-    <row r="266" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -21929,7 +21925,7 @@
         <v>1782.4670000076294</v>
       </c>
     </row>
-    <row r="268" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -22053,7 +22049,7 @@
         <v>1739.8429999351501</v>
       </c>
     </row>
-    <row r="270" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -22115,7 +22111,7 @@
         <v>107.65799999237043</v>
       </c>
     </row>
-    <row r="271" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -22177,7 +22173,7 @@
         <v>107.9489998817437</v>
       </c>
     </row>
-    <row r="272" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -22424,7 +22420,7 @@
         <v>1443.5050001144416</v>
       </c>
     </row>
-    <row r="276" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -22486,7 +22482,7 @@
         <v>738.42399978637138</v>
       </c>
     </row>
-    <row r="277" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -22610,7 +22606,7 @@
         <v>1761.8400001525879</v>
       </c>
     </row>
-    <row r="279" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -22795,7 +22791,7 @@
         <v>1388.2329998016362</v>
       </c>
     </row>
-    <row r="282" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -22856,7 +22852,7 @@
         <v>-1791.5050001144409</v>
       </c>
     </row>
-    <row r="283" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -22918,7 +22914,7 @@
         <v>-16.749000072479248</v>
       </c>
     </row>
-    <row r="284" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -22980,7 +22976,7 @@
         <v>15.499000072479241</v>
       </c>
     </row>
-    <row r="285" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -23042,7 +23038,7 @@
         <v>-248.32999992370543</v>
       </c>
     </row>
-    <row r="286" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -23104,7 +23100,7 @@
         <v>-35.477999925613382</v>
       </c>
     </row>
-    <row r="287" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -23166,7 +23162,7 @@
         <v>2.6069998741150435</v>
       </c>
     </row>
-    <row r="288" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -23228,7 +23224,7 @@
         <v>-703.84800004959072</v>
       </c>
     </row>
-    <row r="289" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -23290,7 +23286,7 @@
         <v>-94.626999855041447</v>
       </c>
     </row>
-    <row r="290" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -23352,7 +23348,7 @@
         <v>-7.2200000286102215</v>
       </c>
     </row>
-    <row r="291" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -23414,7 +23410,7 @@
         <v>-82.357999801635785</v>
       </c>
     </row>
-    <row r="292" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -23475,7 +23471,7 @@
         <v>-1738.3659999370575</v>
       </c>
     </row>
-    <row r="293" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -23537,7 +23533,7 @@
         <v>-1034.485999822607</v>
       </c>
     </row>
-    <row r="294" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -23599,7 +23595,7 @@
         <v>-1181.6399998664815</v>
       </c>
     </row>
-    <row r="295" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -23660,7 +23656,7 @@
         <v>-1440.7890000343323</v>
       </c>
     </row>
-    <row r="296" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -23721,7 +23717,7 @@
         <v>-1739.1229999065399</v>
       </c>
     </row>
-    <row r="297" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -23782,7 +23778,7 @@
         <v>-1410.4200000762942</v>
       </c>
     </row>
-    <row r="298" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -23843,7 +23839,7 @@
         <v>-1743.970999956131</v>
       </c>
     </row>
-    <row r="299" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -23904,7 +23900,7 @@
         <v>-1748.2299997806549</v>
       </c>
     </row>
-    <row r="300" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -23965,7 +23961,7 @@
         <v>-1765.5</v>
       </c>
     </row>
-    <row r="301" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -24026,7 +24022,7 @@
         <v>-1505.8510000705724</v>
       </c>
     </row>
-    <row r="302" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>301</v>
       </c>
@@ -24212,7 +24208,7 @@
         <v>1642.7530000209817</v>
       </c>
     </row>
-    <row r="305" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>304</v>
       </c>
@@ -24274,7 +24270,7 @@
         <v>724.23000001907337</v>
       </c>
     </row>
-    <row r="306" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>305</v>
       </c>
@@ -24398,7 +24394,7 @@
         <v>1359.0490000247958</v>
       </c>
     </row>
-    <row r="308" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>307</v>
       </c>
@@ -24522,7 +24518,7 @@
         <v>1756.2109999656677</v>
       </c>
     </row>
-    <row r="310" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>309</v>
       </c>
@@ -24584,7 +24580,7 @@
         <v>748.85699987411431</v>
       </c>
     </row>
-    <row r="311" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>310</v>
       </c>
@@ -24646,7 +24642,7 @@
         <v>296.09699988365196</v>
       </c>
     </row>
-    <row r="312" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>311</v>
       </c>
@@ -24708,7 +24704,7 @@
         <v>1560.040999889364</v>
       </c>
     </row>
-    <row r="313" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>312</v>
       </c>
@@ -24769,7 +24765,7 @@
         <v>-922.74799990654606</v>
       </c>
     </row>
-    <row r="314" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>313</v>
       </c>
@@ -24831,7 +24827,7 @@
         <v>1148.8599998950917</v>
       </c>
     </row>
-    <row r="315" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>314</v>
       </c>
@@ -24955,7 +24951,7 @@
         <v>1520.0679998397829</v>
       </c>
     </row>
-    <row r="317" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>316</v>
       </c>
@@ -25017,7 +25013,7 @@
         <v>1780.0769999027189</v>
       </c>
     </row>
-    <row r="318" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>317</v>
       </c>
@@ -25140,7 +25136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>319</v>
       </c>
@@ -25265,13 +25261,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S321">
-    <filterColumn colId="17">
-      <filters>
-        <filter val="1800"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S321"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -25281,7 +25271,7 @@
   <dimension ref="A1:Q321"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42124,7 +42114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>

</xml_diff>